<commit_message>
Added valueOrTemplateVariable method to ItemController
</commit_message>
<xml_diff>
--- a/Implementation Status.xlsx
+++ b/Implementation Status.xlsx
@@ -699,9 +699,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>min and max attributes may be variable refs (not implemented)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Class </t>
   </si>
   <si>
@@ -874,6 +871,9 @@
   </si>
   <si>
     <t>Doesn't support weightIdentifier attribute (outside item scope)</t>
+  </si>
+  <si>
+    <t>min and max attributes may be variable refs (not implemented) - FIXED</t>
   </si>
 </sst>
 </file>
@@ -1224,7 +1224,7 @@
   <dimension ref="A1:E215"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B216" sqref="B216"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1326,7 +1326,7 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="C7" t="s">
         <v>224</v>
@@ -1335,7 +1335,7 @@
         <v>222</v>
       </c>
       <c r="E7" t="s">
-        <v>226</v>
+        <v>284</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1346,10 +1346,10 @@
         <v>218</v>
       </c>
       <c r="C8" t="s">
+        <v>226</v>
+      </c>
+      <c r="D8" t="s">
         <v>227</v>
-      </c>
-      <c r="D8" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1360,10 +1360,10 @@
         <v>218</v>
       </c>
       <c r="C9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1371,16 +1371,16 @@
         <v>209</v>
       </c>
       <c r="B10" t="s">
+        <v>229</v>
+      </c>
+      <c r="C10" t="s">
+        <v>229</v>
+      </c>
+      <c r="D10" t="s">
+        <v>229</v>
+      </c>
+      <c r="E10" t="s">
         <v>230</v>
-      </c>
-      <c r="C10" t="s">
-        <v>230</v>
-      </c>
-      <c r="D10" t="s">
-        <v>230</v>
-      </c>
-      <c r="E10" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1388,10 +1388,10 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
+        <v>231</v>
+      </c>
+      <c r="E11" t="s">
         <v>232</v>
-      </c>
-      <c r="E11" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1399,10 +1399,10 @@
         <v>210</v>
       </c>
       <c r="B12" t="s">
+        <v>231</v>
+      </c>
+      <c r="E12" t="s">
         <v>232</v>
-      </c>
-      <c r="E12" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1410,10 +1410,10 @@
         <v>171</v>
       </c>
       <c r="B13" t="s">
+        <v>231</v>
+      </c>
+      <c r="E13" t="s">
         <v>232</v>
-      </c>
-      <c r="E13" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1421,10 +1421,10 @@
         <v>211</v>
       </c>
       <c r="B14" t="s">
+        <v>231</v>
+      </c>
+      <c r="E14" t="s">
         <v>232</v>
-      </c>
-      <c r="E14" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1432,7 +1432,7 @@
         <v>172</v>
       </c>
       <c r="B15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1443,13 +1443,13 @@
         <v>223</v>
       </c>
       <c r="C16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D16" t="s">
         <v>220</v>
       </c>
       <c r="E16" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1477,7 +1477,7 @@
         <v>224</v>
       </c>
       <c r="D18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1527,10 +1527,10 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
+        <v>231</v>
+      </c>
+      <c r="E22" t="s">
         <v>232</v>
-      </c>
-      <c r="E22" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1555,13 +1555,13 @@
         <v>223</v>
       </c>
       <c r="C24" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D24" t="s">
         <v>220</v>
       </c>
       <c r="E24" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1673,10 +1673,10 @@
         <v>224</v>
       </c>
       <c r="D32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E32" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1684,7 +1684,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1692,7 +1692,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1714,16 +1714,16 @@
         <v>177</v>
       </c>
       <c r="B36" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C36" t="s">
         <v>224</v>
       </c>
       <c r="D36" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E36" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1731,16 +1731,16 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
+        <v>238</v>
+      </c>
+      <c r="C37" t="s">
+        <v>226</v>
+      </c>
+      <c r="D37" t="s">
+        <v>234</v>
+      </c>
+      <c r="E37" t="s">
         <v>239</v>
-      </c>
-      <c r="C37" t="s">
-        <v>227</v>
-      </c>
-      <c r="D37" t="s">
-        <v>235</v>
-      </c>
-      <c r="E37" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1754,7 +1754,7 @@
         <v>224</v>
       </c>
       <c r="D38" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1796,7 +1796,7 @@
         <v>224</v>
       </c>
       <c r="D41" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1818,7 +1818,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1840,7 +1840,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1848,7 +1848,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1873,7 +1873,7 @@
         <v>218</v>
       </c>
       <c r="C48" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D48" t="s">
         <v>220</v>
@@ -1884,10 +1884,10 @@
         <v>46</v>
       </c>
       <c r="B49" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E49" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1904,7 +1904,7 @@
         <v>222</v>
       </c>
       <c r="E50" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1912,10 +1912,10 @@
         <v>0</v>
       </c>
       <c r="B51" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E51" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1923,10 +1923,10 @@
         <v>1</v>
       </c>
       <c r="B52" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E52" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1934,10 +1934,10 @@
         <v>2</v>
       </c>
       <c r="B53" t="s">
+        <v>231</v>
+      </c>
+      <c r="E53" t="s">
         <v>232</v>
-      </c>
-      <c r="E53" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1945,16 +1945,16 @@
         <v>48</v>
       </c>
       <c r="B54" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C54" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D54" t="s">
         <v>220</v>
       </c>
       <c r="E54" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1965,7 +1965,7 @@
         <v>218</v>
       </c>
       <c r="C55" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D55" t="s">
         <v>220</v>
@@ -1979,7 +1979,7 @@
         <v>218</v>
       </c>
       <c r="C56" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D56" t="s">
         <v>220</v>
@@ -1990,7 +1990,7 @@
         <v>49</v>
       </c>
       <c r="B57" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2001,13 +2001,13 @@
         <v>223</v>
       </c>
       <c r="C58" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D58" t="s">
         <v>220</v>
       </c>
       <c r="E58" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -2015,7 +2015,7 @@
         <v>50</v>
       </c>
       <c r="B59" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2023,16 +2023,16 @@
         <v>51</v>
       </c>
       <c r="B60" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C60" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D60" t="s">
         <v>220</v>
       </c>
       <c r="E60" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2043,13 +2043,13 @@
         <v>218</v>
       </c>
       <c r="C61" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D61" t="s">
+        <v>247</v>
+      </c>
+      <c r="E61" t="s">
         <v>248</v>
-      </c>
-      <c r="E61" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2057,7 +2057,7 @@
         <v>53</v>
       </c>
       <c r="B62" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2065,7 +2065,7 @@
         <v>54</v>
       </c>
       <c r="B63" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -2073,7 +2073,7 @@
         <v>55</v>
       </c>
       <c r="B64" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -2081,7 +2081,7 @@
         <v>56</v>
       </c>
       <c r="B65" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -2201,7 +2201,7 @@
         <v>180</v>
       </c>
       <c r="B74" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -2209,7 +2209,7 @@
         <v>65</v>
       </c>
       <c r="B75" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -2217,16 +2217,16 @@
         <v>66</v>
       </c>
       <c r="B76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C76" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D76" t="s">
         <v>220</v>
       </c>
       <c r="E76" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -2237,13 +2237,13 @@
         <v>223</v>
       </c>
       <c r="C77" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D77" t="s">
         <v>220</v>
       </c>
       <c r="E77" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -2293,16 +2293,16 @@
         <v>69</v>
       </c>
       <c r="B81" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C81" t="s">
         <v>224</v>
       </c>
       <c r="D81" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E81" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -2310,7 +2310,7 @@
         <v>70</v>
       </c>
       <c r="B82" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -2318,16 +2318,16 @@
         <v>71</v>
       </c>
       <c r="B83" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C83" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D83" t="s">
         <v>220</v>
       </c>
       <c r="E83" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -2335,16 +2335,16 @@
         <v>72</v>
       </c>
       <c r="B84" t="s">
+        <v>253</v>
+      </c>
+      <c r="C84" t="s">
+        <v>226</v>
+      </c>
+      <c r="D84" t="s">
+        <v>220</v>
+      </c>
+      <c r="E84" t="s">
         <v>254</v>
-      </c>
-      <c r="C84" t="s">
-        <v>227</v>
-      </c>
-      <c r="D84" t="s">
-        <v>220</v>
-      </c>
-      <c r="E84" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -2352,7 +2352,7 @@
         <v>73</v>
       </c>
       <c r="B85" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -2360,7 +2360,7 @@
         <v>74</v>
       </c>
       <c r="B86" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C86" t="s">
         <v>224</v>
@@ -2369,7 +2369,7 @@
         <v>220</v>
       </c>
       <c r="E86" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -2377,7 +2377,7 @@
         <v>75</v>
       </c>
       <c r="B87" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C87" t="s">
         <v>224</v>
@@ -2386,7 +2386,7 @@
         <v>220</v>
       </c>
       <c r="E87" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -2408,7 +2408,7 @@
         <v>77</v>
       </c>
       <c r="B89" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -2416,7 +2416,7 @@
         <v>183</v>
       </c>
       <c r="B90" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -2452,10 +2452,10 @@
         <v>184</v>
       </c>
       <c r="B93" t="s">
+        <v>231</v>
+      </c>
+      <c r="E93" t="s">
         <v>232</v>
-      </c>
-      <c r="E93" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -2477,7 +2477,7 @@
         <v>81</v>
       </c>
       <c r="B95" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -2499,7 +2499,7 @@
         <v>82</v>
       </c>
       <c r="B97" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2538,10 +2538,10 @@
         <v>218</v>
       </c>
       <c r="C100" t="s">
+        <v>226</v>
+      </c>
+      <c r="D100" t="s">
         <v>227</v>
-      </c>
-      <c r="D100" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2552,10 +2552,10 @@
         <v>218</v>
       </c>
       <c r="C101" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D101" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -2569,10 +2569,10 @@
         <v>224</v>
       </c>
       <c r="D102" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E102" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -2580,16 +2580,16 @@
         <v>187</v>
       </c>
       <c r="B103" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C103" t="s">
         <v>224</v>
       </c>
       <c r="D103" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E103" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -2603,10 +2603,10 @@
         <v>224</v>
       </c>
       <c r="D104" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E104" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -2617,13 +2617,13 @@
         <v>223</v>
       </c>
       <c r="C105" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D105" t="s">
         <v>220</v>
       </c>
       <c r="E105" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -2631,7 +2631,7 @@
         <v>88</v>
       </c>
       <c r="B106" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -2639,7 +2639,7 @@
         <v>188</v>
       </c>
       <c r="B107" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -2647,10 +2647,10 @@
         <v>189</v>
       </c>
       <c r="B108" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E108" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -2658,7 +2658,7 @@
         <v>89</v>
       </c>
       <c r="B109" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -2666,10 +2666,10 @@
         <v>90</v>
       </c>
       <c r="B110" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E110" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -2677,10 +2677,10 @@
         <v>91</v>
       </c>
       <c r="B111" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E111" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -2702,10 +2702,10 @@
         <v>93</v>
       </c>
       <c r="B113" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E113" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -2716,13 +2716,13 @@
         <v>223</v>
       </c>
       <c r="C114" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D114" t="s">
         <v>220</v>
       </c>
       <c r="E114" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -2736,7 +2736,7 @@
         <v>224</v>
       </c>
       <c r="D115" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -2750,7 +2750,7 @@
         <v>224</v>
       </c>
       <c r="D116" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -2758,10 +2758,10 @@
         <v>190</v>
       </c>
       <c r="B117" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E117" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -2769,10 +2769,10 @@
         <v>191</v>
       </c>
       <c r="B118" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E118" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -2780,10 +2780,10 @@
         <v>192</v>
       </c>
       <c r="B119" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E119" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -2791,10 +2791,10 @@
         <v>193</v>
       </c>
       <c r="B120" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E120" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -2802,10 +2802,10 @@
         <v>194</v>
       </c>
       <c r="B121" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E121" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -2841,16 +2841,16 @@
         <v>99</v>
       </c>
       <c r="B124" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C124" t="s">
         <v>224</v>
       </c>
       <c r="D124" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E124" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
@@ -2864,10 +2864,10 @@
         <v>224</v>
       </c>
       <c r="D125" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E125" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -2875,10 +2875,10 @@
         <v>101</v>
       </c>
       <c r="B126" t="s">
+        <v>231</v>
+      </c>
+      <c r="E126" t="s">
         <v>232</v>
-      </c>
-      <c r="E126" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -2889,13 +2889,13 @@
         <v>223</v>
       </c>
       <c r="C127" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D127" t="s">
         <v>220</v>
       </c>
       <c r="E127" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -2903,10 +2903,10 @@
         <v>103</v>
       </c>
       <c r="B128" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E128" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -2914,10 +2914,10 @@
         <v>212</v>
       </c>
       <c r="B129" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E129" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -2925,10 +2925,10 @@
         <v>104</v>
       </c>
       <c r="B130" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E130" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -2936,10 +2936,10 @@
         <v>105</v>
       </c>
       <c r="B131" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E131" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -2947,10 +2947,10 @@
         <v>106</v>
       </c>
       <c r="B132" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E132" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -2958,10 +2958,10 @@
         <v>195</v>
       </c>
       <c r="B133" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E133" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -2969,10 +2969,10 @@
         <v>196</v>
       </c>
       <c r="B134" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E134" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -2980,10 +2980,10 @@
         <v>107</v>
       </c>
       <c r="B135" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E135" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -2991,10 +2991,10 @@
         <v>108</v>
       </c>
       <c r="B136" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E136" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -3025,7 +3025,7 @@
         <v>220</v>
       </c>
       <c r="E138" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -3033,16 +3033,16 @@
         <v>110</v>
       </c>
       <c r="B139" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C139" t="s">
         <v>224</v>
       </c>
       <c r="D139" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E139" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -3050,7 +3050,7 @@
         <v>111</v>
       </c>
       <c r="B140" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -3058,7 +3058,7 @@
         <v>112</v>
       </c>
       <c r="B141" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -3072,7 +3072,7 @@
         <v>224</v>
       </c>
       <c r="D142" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -3094,10 +3094,10 @@
         <v>115</v>
       </c>
       <c r="B144" t="s">
+        <v>231</v>
+      </c>
+      <c r="E144" t="s">
         <v>232</v>
-      </c>
-      <c r="E144" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -3114,7 +3114,7 @@
         <v>220</v>
       </c>
       <c r="E145" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -3128,7 +3128,7 @@
         <v>224</v>
       </c>
       <c r="D146" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -3139,13 +3139,13 @@
         <v>218</v>
       </c>
       <c r="C147" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D147" t="s">
         <v>220</v>
       </c>
       <c r="E147" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
@@ -3187,10 +3187,10 @@
         <v>224</v>
       </c>
       <c r="D150" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E150" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -3204,10 +3204,10 @@
         <v>224</v>
       </c>
       <c r="D151" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E151" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -3215,7 +3215,7 @@
         <v>120</v>
       </c>
       <c r="B152" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -3229,7 +3229,7 @@
         <v>224</v>
       </c>
       <c r="D153" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -3240,10 +3240,10 @@
         <v>218</v>
       </c>
       <c r="C154" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D154" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -3257,7 +3257,7 @@
         <v>224</v>
       </c>
       <c r="D155" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -3271,7 +3271,7 @@
         <v>224</v>
       </c>
       <c r="D156" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -3285,7 +3285,7 @@
         <v>224</v>
       </c>
       <c r="D157" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
@@ -3299,7 +3299,7 @@
         <v>224</v>
       </c>
       <c r="D158" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -3307,7 +3307,7 @@
         <v>123</v>
       </c>
       <c r="B159" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -3321,7 +3321,7 @@
         <v>224</v>
       </c>
       <c r="D160" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -3329,7 +3329,7 @@
         <v>125</v>
       </c>
       <c r="B161" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -3337,7 +3337,7 @@
         <v>126</v>
       </c>
       <c r="B162" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
@@ -3359,10 +3359,10 @@
         <v>128</v>
       </c>
       <c r="B164" t="s">
+        <v>231</v>
+      </c>
+      <c r="E164" t="s">
         <v>232</v>
-      </c>
-      <c r="E164" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
@@ -3373,13 +3373,13 @@
         <v>223</v>
       </c>
       <c r="C165" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D165" t="s">
         <v>220</v>
       </c>
       <c r="E165" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
@@ -3393,7 +3393,7 @@
         <v>224</v>
       </c>
       <c r="D166" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -3407,7 +3407,7 @@
         <v>224</v>
       </c>
       <c r="D167" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
@@ -3421,7 +3421,7 @@
         <v>224</v>
       </c>
       <c r="D168" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
@@ -3435,7 +3435,7 @@
         <v>224</v>
       </c>
       <c r="D169" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
@@ -3446,13 +3446,13 @@
         <v>223</v>
       </c>
       <c r="C170" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D170" t="s">
         <v>220</v>
       </c>
       <c r="E170" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -3460,16 +3460,16 @@
         <v>135</v>
       </c>
       <c r="B171" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C171" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D171" t="s">
         <v>220</v>
       </c>
       <c r="E171" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -3477,16 +3477,16 @@
         <v>136</v>
       </c>
       <c r="B172" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C172" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D172" t="s">
+        <v>275</v>
+      </c>
+      <c r="E172" t="s">
         <v>276</v>
-      </c>
-      <c r="E172" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
@@ -3497,13 +3497,13 @@
         <v>223</v>
       </c>
       <c r="C173" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D173" t="s">
         <v>220</v>
       </c>
       <c r="E173" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -3539,7 +3539,7 @@
         <v>140</v>
       </c>
       <c r="B176" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
@@ -3547,7 +3547,7 @@
         <v>141</v>
       </c>
       <c r="B177" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C177" t="s">
         <v>224</v>
@@ -3556,7 +3556,7 @@
         <v>220</v>
       </c>
       <c r="E177" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -3581,7 +3581,7 @@
         <v>218</v>
       </c>
       <c r="C179" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
@@ -3609,7 +3609,7 @@
         <v>224</v>
       </c>
       <c r="D181" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
@@ -3623,7 +3623,7 @@
         <v>224</v>
       </c>
       <c r="D182" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
@@ -3637,7 +3637,7 @@
         <v>224</v>
       </c>
       <c r="D183" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
@@ -3701,7 +3701,7 @@
         <v>4</v>
       </c>
       <c r="B188" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
@@ -3715,7 +3715,7 @@
         <v>224</v>
       </c>
       <c r="D189" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
@@ -3723,7 +3723,7 @@
         <v>152</v>
       </c>
       <c r="B190" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
@@ -3737,7 +3737,7 @@
         <v>224</v>
       </c>
       <c r="D191" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
@@ -3745,7 +3745,7 @@
         <v>154</v>
       </c>
       <c r="B192" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
@@ -3759,7 +3759,7 @@
         <v>221</v>
       </c>
       <c r="D193" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
@@ -3767,13 +3767,13 @@
         <v>156</v>
       </c>
       <c r="B194" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C194" t="s">
         <v>224</v>
       </c>
       <c r="D194" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
@@ -3781,13 +3781,13 @@
         <v>157</v>
       </c>
       <c r="B195" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C195" t="s">
         <v>224</v>
       </c>
       <c r="D195" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
@@ -3795,7 +3795,7 @@
         <v>5</v>
       </c>
       <c r="B196" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
@@ -3809,7 +3809,7 @@
         <v>224</v>
       </c>
       <c r="D197" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
@@ -3817,10 +3817,10 @@
         <v>159</v>
       </c>
       <c r="B198" t="s">
+        <v>231</v>
+      </c>
+      <c r="E198" t="s">
         <v>232</v>
-      </c>
-      <c r="E198" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
@@ -3828,10 +3828,10 @@
         <v>160</v>
       </c>
       <c r="B199" t="s">
+        <v>231</v>
+      </c>
+      <c r="E199" t="s">
         <v>232</v>
-      </c>
-      <c r="E199" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
@@ -3839,10 +3839,10 @@
         <v>202</v>
       </c>
       <c r="B200" t="s">
+        <v>231</v>
+      </c>
+      <c r="E200" t="s">
         <v>232</v>
-      </c>
-      <c r="E200" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -3853,13 +3853,13 @@
         <v>223</v>
       </c>
       <c r="C201" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D201" t="s">
         <v>220</v>
       </c>
       <c r="E201" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
@@ -3909,10 +3909,10 @@
         <v>204</v>
       </c>
       <c r="B205" t="s">
+        <v>231</v>
+      </c>
+      <c r="E205" t="s">
         <v>232</v>
-      </c>
-      <c r="E205" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
@@ -3940,7 +3940,7 @@
         <v>224</v>
       </c>
       <c r="D207" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
@@ -3979,7 +3979,7 @@
         <v>218</v>
       </c>
       <c r="C210" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D210" t="s">
         <v>220</v>
@@ -3990,16 +3990,16 @@
         <v>205</v>
       </c>
       <c r="B211" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C211" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D211" t="s">
         <v>220</v>
       </c>
       <c r="E211" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
@@ -4027,10 +4027,10 @@
         <v>221</v>
       </c>
       <c r="D213" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E213" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
@@ -4038,7 +4038,7 @@
         <v>207</v>
       </c>
       <c r="B214" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
@@ -4046,7 +4046,7 @@
         <v>208</v>
       </c>
       <c r="B215" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated status (max implemented)
</commit_message>
<xml_diff>
--- a/Implementation Status.xlsx
+++ b/Implementation Status.xlsx
@@ -15,7 +15,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$215</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -1222,10 +1221,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
-      <selection activeCell="B211" sqref="B211"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="E110" sqref="E110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1252,7 +1252,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>170</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>210</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>171</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>211</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>173</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>174</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1534,7 +1534,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1593,7 +1593,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>175</v>
       </c>
@@ -1607,7 +1607,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>176</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1687,6 +1687,9 @@
       <c r="B33" t="s">
         <v>231</v>
       </c>
+      <c r="E33" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -1695,8 +1698,11 @@
       <c r="B34" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1710,7 +1716,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>177</v>
       </c>
@@ -1727,7 +1733,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1744,7 +1750,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1758,7 +1764,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1772,7 +1778,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1786,7 +1792,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1800,7 +1806,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1822,7 +1828,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1852,7 +1858,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -1866,7 +1872,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>178</v>
       </c>
@@ -1891,7 +1897,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>47</v>
       </c>
@@ -1930,7 +1936,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>2</v>
       </c>
@@ -1958,7 +1964,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>3</v>
       </c>
@@ -1972,7 +1978,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>6</v>
       </c>
@@ -1986,15 +1992,15 @@
         <v>220</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>49</v>
       </c>
       <c r="B57" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>179</v>
       </c>
@@ -2036,7 +2042,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>52</v>
       </c>
@@ -2053,12 +2059,12 @@
         <v>245</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>53</v>
       </c>
       <c r="B62" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2085,7 +2091,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>57</v>
       </c>
@@ -2099,7 +2105,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>58</v>
       </c>
@@ -2113,7 +2119,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>59</v>
       </c>
@@ -2127,7 +2133,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>60</v>
       </c>
@@ -2141,7 +2147,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>61</v>
       </c>
@@ -2155,7 +2161,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>62</v>
       </c>
@@ -2169,7 +2175,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>63</v>
       </c>
@@ -2183,7 +2189,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>64</v>
       </c>
@@ -2247,7 +2253,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>181</v>
       </c>
@@ -2261,7 +2267,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>68</v>
       </c>
@@ -2275,7 +2281,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>182</v>
       </c>
@@ -2289,7 +2295,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>69</v>
       </c>
@@ -2356,7 +2362,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>74</v>
       </c>
@@ -2373,7 +2379,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>75</v>
       </c>
@@ -2390,7 +2396,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>76</v>
       </c>
@@ -2420,7 +2426,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>78</v>
       </c>
@@ -2434,7 +2440,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>79</v>
       </c>
@@ -2448,7 +2454,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>184</v>
       </c>
@@ -2459,7 +2465,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>80</v>
       </c>
@@ -2473,15 +2479,15 @@
         <v>220</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>81</v>
       </c>
       <c r="B95" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>7</v>
       </c>
@@ -2503,7 +2509,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>83</v>
       </c>
@@ -2517,7 +2523,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>84</v>
       </c>
@@ -2531,7 +2537,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>185</v>
       </c>
@@ -2545,7 +2551,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>85</v>
       </c>
@@ -2593,7 +2599,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>86</v>
       </c>
@@ -2648,10 +2654,7 @@
         <v>189</v>
       </c>
       <c r="B108" t="s">
-        <v>231</v>
-      </c>
-      <c r="E108" t="s">
-        <v>254</v>
+        <v>218</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -2667,10 +2670,7 @@
         <v>90</v>
       </c>
       <c r="B110" t="s">
-        <v>231</v>
-      </c>
-      <c r="E110" t="s">
-        <v>254</v>
+        <v>218</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -2684,7 +2684,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>92</v>
       </c>
@@ -2726,7 +2726,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>95</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>96</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>190</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>191</v>
       </c>
@@ -2776,7 +2776,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>192</v>
       </c>
@@ -2787,7 +2787,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>193</v>
       </c>
@@ -2798,7 +2798,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>194</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>97</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>98</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>99</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>100</v>
       </c>
@@ -2871,7 +2871,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>101</v>
       </c>
@@ -2899,7 +2899,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>103</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>104</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>105</v>
       </c>
@@ -2943,7 +2943,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>106</v>
       </c>
@@ -2954,7 +2954,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>195</v>
       </c>
@@ -2965,7 +2965,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>196</v>
       </c>
@@ -2976,7 +2976,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>107</v>
       </c>
@@ -2987,7 +2987,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>108</v>
       </c>
@@ -2998,7 +2998,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>109</v>
       </c>
@@ -3029,7 +3029,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>110</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>113</v>
       </c>
@@ -3076,7 +3076,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>114</v>
       </c>
@@ -3090,7 +3090,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>115</v>
       </c>
@@ -3118,7 +3118,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>116</v>
       </c>
@@ -3132,7 +3132,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>117</v>
       </c>
@@ -3149,7 +3149,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>118</v>
       </c>
@@ -3163,7 +3163,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>119</v>
       </c>
@@ -3219,7 +3219,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>121</v>
       </c>
@@ -3233,7 +3233,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>122</v>
       </c>
@@ -3247,7 +3247,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>10</v>
       </c>
@@ -3261,7 +3261,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>9</v>
       </c>
@@ -3275,7 +3275,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>8</v>
       </c>
@@ -3289,7 +3289,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>213</v>
       </c>
@@ -3311,7 +3311,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>124</v>
       </c>
@@ -3341,7 +3341,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>127</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>128</v>
       </c>
@@ -3383,7 +3383,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>130</v>
       </c>
@@ -3397,7 +3397,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>131</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>132</v>
       </c>
@@ -3425,7 +3425,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>133</v>
       </c>
@@ -3507,7 +3507,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>138</v>
       </c>
@@ -3521,7 +3521,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>139</v>
       </c>
@@ -3543,7 +3543,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>141</v>
       </c>
@@ -3560,7 +3560,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>142</v>
       </c>
@@ -3574,7 +3574,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>201</v>
       </c>
@@ -3585,7 +3585,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>143</v>
       </c>
@@ -3599,7 +3599,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>144</v>
       </c>
@@ -3613,7 +3613,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>145</v>
       </c>
@@ -3627,7 +3627,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>146</v>
       </c>
@@ -3641,7 +3641,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>147</v>
       </c>
@@ -3655,7 +3655,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>148</v>
       </c>
@@ -3669,7 +3669,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>149</v>
       </c>
@@ -3683,7 +3683,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>150</v>
       </c>
@@ -3705,7 +3705,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>151</v>
       </c>
@@ -3727,7 +3727,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>153</v>
       </c>
@@ -3749,7 +3749,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>155</v>
       </c>
@@ -3763,7 +3763,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>156</v>
       </c>
@@ -3777,7 +3777,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>157</v>
       </c>
@@ -3799,7 +3799,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>158</v>
       </c>
@@ -3813,7 +3813,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>159</v>
       </c>
@@ -3824,7 +3824,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>160</v>
       </c>
@@ -3835,7 +3835,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>202</v>
       </c>
@@ -3863,7 +3863,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>161</v>
       </c>
@@ -3877,7 +3877,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>162</v>
       </c>
@@ -3891,7 +3891,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>163</v>
       </c>
@@ -3905,7 +3905,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>204</v>
       </c>
@@ -3916,7 +3916,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>164</v>
       </c>
@@ -3930,7 +3930,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>165</v>
       </c>
@@ -3944,7 +3944,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>166</v>
       </c>
@@ -3958,7 +3958,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>167</v>
       </c>
@@ -3972,7 +3972,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>168</v>
       </c>
@@ -4003,7 +4003,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>169</v>
       </c>
@@ -4051,6 +4051,50 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E215">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="?"/>
+        <filter val="Buggy"/>
+        <filter val="None"/>
+        <filter val="Partial"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="4">
+      <filters blank="1">
+        <filter val="Attributes not implemented"/>
+        <filter val="Didn't understand the tolerance attribute but now get it"/>
+        <filter val="Does this display the gaps interleaved with the other content properly?"/>
+        <filter val="Doesn’t implement &quot;title&quot;"/>
+        <filter val="Doesn't do template substitution"/>
+        <filter val="Doesn't implement attributes, although passed to JS"/>
+        <filter val="Doesn't implement choice functionality"/>
+        <filter val="Doesn't implement lowerBound or upperBound"/>
+        <filter val="Doesn't implement lowerBound or upperBound, algorithm may be wrong"/>
+        <filter val="Doesn't implement matchMax and matchMin"/>
+        <filter val="Doesn't implement maxAssociations or minAssociations"/>
+        <filter val="Doesn't implement maxChoices or minChoices"/>
+        <filter val="Doesn't implement minChoices, maxChoices or orientation"/>
+        <filter val="Doesn't implement required [FIXED - implemented required, may still be buggy]"/>
+        <filter val="Doesn't implement templates"/>
+        <filter val="Doesn't implement underlying &quot;choice&quot;"/>
+        <filter val="Doesn't implement underlying &quot;choice&quot; or variable substitution"/>
+        <filter val="Doesn't support most attributes or variable types"/>
+        <filter val="Doesn't support weightIdentifier attribute (outside item scope)"/>
+        <filter val="How to implement this? Maybe an exception would work."/>
+        <filter val="implemented as item controller - should it be element on its own?"/>
+        <filter val="Looks completely wrong"/>
+        <filter val="maxChoices, minChoices not supported in JS"/>
+        <filter val="maxChoices, minChoices not supported in JS, orientation not supported at all"/>
+        <filter val="minAssociations not supported, simpleAssociableChoice not fully supported etc."/>
+        <filter val="No attributes supported"/>
+        <filter val="No intention ever to implement this"/>
+        <filter val="Not sure how this is meant to work"/>
+        <filter val="Only supports single string - no attributes supported"/>
+        <filter val="Should be a quick implementation"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A1:A216">
     <sortCondition ref="A1"/>
   </sortState>

</xml_diff>

<commit_message>
Implemented some more elements
</commit_message>
<xml_diff>
--- a/Implementation Status.xlsx
+++ b/Implementation Status.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="282">
   <si>
     <t>exitResponse</t>
   </si>
@@ -862,6 +862,9 @@
   </si>
   <si>
     <t>Assumes optional substring element is present [FIXED]</t>
+  </si>
+  <si>
+    <t>Only 4 operators implemented</t>
   </si>
 </sst>
 </file>
@@ -1212,8 +1215,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:E215"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="E190" sqref="E190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2641,7 +2644,10 @@
         <v>89</v>
       </c>
       <c r="B109" t="s">
-        <v>231</v>
+        <v>223</v>
+      </c>
+      <c r="E109" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="110" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -3300,7 +3306,7 @@
         <v>125</v>
       </c>
       <c r="B161" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -3694,7 +3700,7 @@
         <v>152</v>
       </c>
       <c r="B190" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
     </row>
     <row r="191" spans="1:5" hidden="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated status - implemented repeat
</commit_message>
<xml_diff>
--- a/Implementation Status.xlsx
+++ b/Implementation Status.xlsx
@@ -7,19 +7,19 @@
     <workbookView xWindow="0" yWindow="2445" windowWidth="10935" windowHeight="6750"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Dev issues" sheetId="1" r:id="rId1"/>
+    <sheet name="Spec issues" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$215</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Dev issues'!$A$1:$F$215</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="285">
   <si>
     <t>exitResponse</t>
   </si>
@@ -871,6 +871,9 @@
   </si>
   <si>
     <t>Doesn't do proper serialisation of template values</t>
+  </si>
+  <si>
+    <t>"The repeat operator takes 0 or more sub-expressions" - result type undefined if zero. Appears to be 1 or more in XSD.</t>
   </si>
 </sst>
 </file>
@@ -1221,8 +1224,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="F138" sqref="F138"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B152" sqref="B152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1368,7 +1371,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>209</v>
       </c>
@@ -1549,7 +1552,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1835,7 +1838,10 @@
         <v>230</v>
       </c>
       <c r="C43">
-        <v>3</v>
+        <v>300000</v>
+      </c>
+      <c r="F43" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -2730,12 +2736,15 @@
         <v>218</v>
       </c>
     </row>
-    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>89</v>
       </c>
       <c r="B109" t="s">
         <v>223</v>
+      </c>
+      <c r="C109">
+        <v>1</v>
       </c>
       <c r="F109" t="s">
         <v>276</v>
@@ -3304,7 +3313,7 @@
         <v>120</v>
       </c>
       <c r="B152" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="C152">
         <v>1</v>
@@ -4201,8 +4210,7 @@
         <filter val="Attributes not implemented"/>
         <filter val="Does this display the gaps interleaved with the other content properly?"/>
         <filter val="Doesn’t implement &quot;title&quot;"/>
-        <filter val="Doesn't do template substitution"/>
-        <filter val="Doesn't implement attributes, although passed to JS"/>
+        <filter val="Doesn't do proper serialisation of template values"/>
         <filter val="Doesn't implement choice functionality"/>
         <filter val="Doesn't implement lowerBound or upperBound"/>
         <filter val="Doesn't implement lowerBound or upperBound, algorithm may be wrong"/>
@@ -4211,18 +4219,21 @@
         <filter val="Doesn't implement maxChoices or minChoices"/>
         <filter val="Doesn't implement minChoices, maxChoices or orientation"/>
         <filter val="Doesn't implement required [FIXED - implemented required, may still be buggy]"/>
+        <filter val="Doesn't implement stepLabel or reverse although passed to JS"/>
         <filter val="Doesn't implement underlying &quot;choice&quot;"/>
         <filter val="Doesn't implement underlying &quot;choice&quot; or variable substitution"/>
         <filter val="Doesn't support most attributes or variable types"/>
+        <filter val="Doesn't support stringInteraction features or other attributes"/>
         <filter val="Doesn't support weightIdentifier attribute (outside item scope)"/>
+        <filter val="implemented as item controller - should it be element on its own? [YES!]"/>
         <filter val="Looks completely wrong"/>
         <filter val="maxChoices, minChoices not supported in JS"/>
-        <filter val="maxChoices, minChoices not supported in JS, orientation not supported at all"/>
         <filter val="minAssociations not supported, simpleAssociableChoice not fully supported etc."/>
         <filter val="No attributes supported"/>
         <filter val="No intention ever to implement this"/>
         <filter val="Not sure how this is meant to work"/>
-        <filter val="Only supports single string - no attributes supported"/>
+        <filter val="Only 4 operators implemented"/>
+        <filter val="Should be easy enough to implement"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -4241,7 +4252,13 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Updated status for statsOperator
</commit_message>
<xml_diff>
--- a/Implementation Status.xlsx
+++ b/Implementation Status.xlsx
@@ -1210,7 +1210,7 @@
   <dimension ref="A1:E215"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="D165" sqref="D165"/>
+      <selection activeCell="B176" sqref="B176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3310,7 +3310,7 @@
         <v>140</v>
       </c>
       <c r="B176" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="C176">
         <v>2</v>

</xml_diff>

<commit_message>
Updated implementation status (mathOperator)
</commit_message>
<xml_diff>
--- a/Implementation Status.xlsx
+++ b/Implementation Status.xlsx
@@ -720,9 +720,6 @@
     <t>Rounding of significantFigures needs futher testing</t>
   </si>
   <si>
-    <t>Does this display the gaps interleaved with the other content properly?</t>
-  </si>
-  <si>
     <t>Null</t>
   </si>
   <si>
@@ -795,9 +792,6 @@
     <t>No attributes supported</t>
   </si>
   <si>
-    <t>Not sure how this is meant to work</t>
-  </si>
-  <si>
     <t>Doesn't support weightIdentifier attribute (outside item scope)</t>
   </si>
   <si>
@@ -831,9 +825,6 @@
     <t>Assumes optional substring element is present [FIXED]</t>
   </si>
   <si>
-    <t>Only 4 operators implemented</t>
-  </si>
-  <si>
     <t>Should be easy enough to implement</t>
   </si>
   <si>
@@ -859,6 +850,15 @@
   </si>
   <si>
     <t>Only supports basic showing hiding via view attribute</t>
+  </si>
+  <si>
+    <t>Does this display the gaps interleaved with the other content properly? [Yes]</t>
+  </si>
+  <si>
+    <t>baseType and fieldIdentifier not implemented</t>
+  </si>
+  <si>
+    <t>Only 17 operators implemented</t>
   </si>
 </sst>
 </file>
@@ -1209,8 +1209,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:E215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B176" sqref="B176"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="E109" sqref="E109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1229,7 +1229,7 @@
         <v>215</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>216</v>
@@ -1304,7 +1304,7 @@
         <v>219</v>
       </c>
       <c r="E7" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -1340,7 +1340,7 @@
         <v>224</v>
       </c>
       <c r="E10" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -1497,7 +1497,7 @@
         <v>218</v>
       </c>
       <c r="E24" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -1602,7 +1602,7 @@
         <v>300000</v>
       </c>
       <c r="E33" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1616,7 +1616,7 @@
         <v>300000</v>
       </c>
       <c r="E34" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -1641,7 +1641,7 @@
         <v>228</v>
       </c>
       <c r="E36" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -1655,7 +1655,7 @@
         <v>228</v>
       </c>
       <c r="E37" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -1724,7 +1724,7 @@
         <v>300000</v>
       </c>
       <c r="E43" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -1845,7 +1845,7 @@
         <v>218</v>
       </c>
       <c r="E54" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -1889,7 +1889,7 @@
         <v>218</v>
       </c>
       <c r="E58" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1917,7 +1917,7 @@
         <v>218</v>
       </c>
       <c r="E60" t="s">
-        <v>233</v>
+        <v>277</v>
       </c>
     </row>
     <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -1928,10 +1928,10 @@
         <v>217</v>
       </c>
       <c r="D61" t="s">
+        <v>233</v>
+      </c>
+      <c r="E61" t="s">
         <v>234</v>
-      </c>
-      <c r="E61" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -2099,7 +2099,7 @@
         <v>218</v>
       </c>
       <c r="E76" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -2116,7 +2116,7 @@
         <v>218</v>
       </c>
       <c r="E77" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -2163,7 +2163,7 @@
         <v>228</v>
       </c>
       <c r="E81" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -2191,7 +2191,7 @@
         <v>218</v>
       </c>
       <c r="E83" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -2208,7 +2208,7 @@
         <v>218</v>
       </c>
       <c r="E84" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -2233,7 +2233,7 @@
         <v>218</v>
       </c>
       <c r="E86" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -2247,7 +2247,7 @@
         <v>218</v>
       </c>
       <c r="E87" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -2398,7 +2398,7 @@
         <v>217</v>
       </c>
       <c r="D101" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -2415,7 +2415,7 @@
         <v>228</v>
       </c>
       <c r="E102" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -2432,7 +2432,7 @@
         <v>228</v>
       </c>
       <c r="E103" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="104" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -2446,7 +2446,7 @@
         <v>228</v>
       </c>
       <c r="E104" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -2463,7 +2463,7 @@
         <v>218</v>
       </c>
       <c r="E105" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -2507,7 +2507,7 @@
         <v>1</v>
       </c>
       <c r="E109" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
     </row>
     <row r="110" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -2529,7 +2529,7 @@
         <v>300000</v>
       </c>
       <c r="E111" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="112" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -2562,7 +2562,7 @@
         <v>218</v>
       </c>
       <c r="E114" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="115" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -2595,7 +2595,7 @@
         <v>225</v>
       </c>
       <c r="E117" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="118" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -2606,7 +2606,7 @@
         <v>225</v>
       </c>
       <c r="E118" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="119" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -2617,7 +2617,7 @@
         <v>225</v>
       </c>
       <c r="E119" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="120" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -2628,7 +2628,7 @@
         <v>225</v>
       </c>
       <c r="E120" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="121" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -2639,7 +2639,7 @@
         <v>225</v>
       </c>
       <c r="E121" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="122" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -2675,7 +2675,7 @@
         <v>228</v>
       </c>
       <c r="E124" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="125" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -2689,7 +2689,7 @@
         <v>228</v>
       </c>
       <c r="E125" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="126" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -2717,7 +2717,7 @@
         <v>218</v>
       </c>
       <c r="E127" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="128" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -2728,7 +2728,7 @@
         <v>225</v>
       </c>
       <c r="E128" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -2742,7 +2742,7 @@
         <v>1</v>
       </c>
       <c r="E129" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="130" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -2753,7 +2753,7 @@
         <v>225</v>
       </c>
       <c r="E130" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="131" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -2764,7 +2764,7 @@
         <v>225</v>
       </c>
       <c r="E131" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="132" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -2775,7 +2775,7 @@
         <v>225</v>
       </c>
       <c r="E132" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="133" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -2786,7 +2786,7 @@
         <v>225</v>
       </c>
       <c r="E133" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="134" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -2797,7 +2797,7 @@
         <v>225</v>
       </c>
       <c r="E134" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="135" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -2808,7 +2808,7 @@
         <v>225</v>
       </c>
       <c r="E135" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="136" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -2819,7 +2819,7 @@
         <v>225</v>
       </c>
       <c r="E136" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="137" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -2847,7 +2847,7 @@
         <v>218</v>
       </c>
       <c r="E138" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="139" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -2861,7 +2861,7 @@
         <v>228</v>
       </c>
       <c r="E139" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -2933,7 +2933,7 @@
         <v>218</v>
       </c>
       <c r="E145" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="146" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -2958,7 +2958,7 @@
         <v>218</v>
       </c>
       <c r="E147" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="148" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -3016,7 +3016,7 @@
         <v>1</v>
       </c>
       <c r="E152" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="153" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -3129,7 +3129,7 @@
         <v>218</v>
       </c>
       <c r="E162" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="163" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -3168,7 +3168,7 @@
         <v>218</v>
       </c>
       <c r="E165" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="166" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -3229,7 +3229,7 @@
         <v>218</v>
       </c>
       <c r="E170" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -3246,7 +3246,7 @@
         <v>218</v>
       </c>
       <c r="E171" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -3260,10 +3260,10 @@
         <v>2</v>
       </c>
       <c r="D172" t="s">
+        <v>253</v>
+      </c>
+      <c r="E172" t="s">
         <v>254</v>
-      </c>
-      <c r="E172" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
@@ -3280,7 +3280,7 @@
         <v>218</v>
       </c>
       <c r="E173" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="174" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -3327,7 +3327,7 @@
         <v>218</v>
       </c>
       <c r="E177" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="178" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -3502,7 +3502,7 @@
         <v>156</v>
       </c>
       <c r="B194" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D194" t="s">
         <v>225</v>
@@ -3513,7 +3513,7 @@
         <v>157</v>
       </c>
       <c r="B195" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D195" t="s">
         <v>225</v>
@@ -3585,7 +3585,7 @@
         <v>218</v>
       </c>
       <c r="E201" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="202" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -3701,7 +3701,7 @@
         <v>218</v>
       </c>
       <c r="E211" t="s">
-        <v>258</v>
+        <v>278</v>
       </c>
     </row>
     <row r="212" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -3729,7 +3729,7 @@
         <v>228</v>
       </c>
       <c r="E213" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="214" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -3814,7 +3814,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated status for mathOperator
</commit_message>
<xml_diff>
--- a/Implementation Status.xlsx
+++ b/Implementation Status.xlsx
@@ -858,7 +858,7 @@
     <t>baseType and fieldIdentifier not implemented</t>
   </si>
   <si>
-    <t>3 operators unimplemented</t>
+    <t>All operators implemented - most untested</t>
   </si>
 </sst>
 </file>
@@ -1209,8 +1209,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:E215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="E111" sqref="E111"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1329,12 +1329,12 @@
         <v>223</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>209</v>
       </c>
       <c r="B10" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="D10" t="s">
         <v>224</v>
@@ -1903,7 +1903,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>51</v>
       </c>
@@ -2496,12 +2496,12 @@
         <v>217</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>89</v>
       </c>
       <c r="B109" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C109">
         <v>1</v>
@@ -3115,7 +3115,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>126</v>
       </c>
@@ -3305,7 +3305,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>140</v>
       </c>
@@ -3687,7 +3687,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>205</v>
       </c>
@@ -3758,7 +3758,6 @@
   <autoFilter ref="A1:E215">
     <filterColumn colId="1">
       <filters>
-        <filter val="?"/>
         <filter val="Buggy"/>
         <filter val="None"/>
         <filter val="Partial"/>

</xml_diff>